<commit_message>
nop bai tap test case full
</commit_message>
<xml_diff>
--- a/assignment/tran-quang-lam/assignment-webui/Data Files/Excel files/quan-ly-san-pham-va-gio-hang.xlsx
+++ b/assignment/tran-quang-lam/assignment-webui/Data Files/Excel files/quan-ly-san-pham-va-gio-hang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\katalon\assignment\tran-quang-lam\assignment-webui\Data Files\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCB4AB8-5D7C-4E4C-BC49-0728B2FCE7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116145FA-7990-4398-AEAF-F58AB1BDA594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{595C574F-D71C-4844-BA6E-D6AFBE824FF0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>searchName</t>
   </si>
@@ -504,7 +504,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,9 +595,6 @@
       <c r="B9" t="s">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
       <c r="F9" s="2" t="s">
         <v>20</v>
       </c>

</xml_diff>